<commit_message>
change sanger to sequencing file
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -2552,7 +2552,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Sanger sequencing"</formula1>
+      <formula1>"Sequencing file"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2603,7 +2603,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Sanger sequencing"</formula1>
+      <formula1>"Sequencing file"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
change sanger to sequencing file (#35)
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -2552,7 +2552,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Sanger sequencing"</formula1>
+      <formula1>"Sequencing file"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2603,7 +2603,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Sanger sequencing"</formula1>
+      <formula1>"Sequencing file"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add database_id fields (#36)
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -481,7 +481,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,6 +532,11 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -547,7 +552,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -597,6 +602,11 @@
         </is>
       </c>
       <c r="I1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -618,7 +628,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -658,6 +668,11 @@
         </is>
       </c>
       <c r="G1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -679,7 +694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -729,6 +744,11 @@
         </is>
       </c>
       <c r="I1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -753,7 +773,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -798,6 +818,11 @@
         </is>
       </c>
       <c r="H1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -819,7 +844,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -864,6 +889,11 @@
         </is>
       </c>
       <c r="H1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -885,7 +915,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -925,6 +955,11 @@
         </is>
       </c>
       <c r="G1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -946,7 +981,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -986,6 +1021,11 @@
         </is>
       </c>
       <c r="G1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1007,7 +1047,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1047,6 +1087,11 @@
         </is>
       </c>
       <c r="G1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1068,7 +1113,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1113,6 +1158,11 @@
         </is>
       </c>
       <c r="H1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1175,7 +1225,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1241,6 +1291,11 @@
       </c>
       <c r="L1" t="inlineStr">
         <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -1256,7 +1311,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1297,6 +1352,11 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -1312,7 +1372,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1353,6 +1413,11 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -1445,7 +1510,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1486,6 +1551,11 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -1501,6 +1571,72 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>add_primer_features</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1512,39 +1648,100 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>add_primer_features</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>assembly</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>input</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>type</t>
+          <t>output_name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>output_name</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
       <c r="H1" t="inlineStr">
         <is>
           <t>id</t>
@@ -1556,13 +1753,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1603,117 +1800,10 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1786,7 +1876,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1827,6 +1917,11 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -1842,7 +1937,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1883,6 +1978,11 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -1898,7 +1998,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1944,6 +2044,11 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -1959,7 +2064,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2009,6 +2114,11 @@
         </is>
       </c>
       <c r="I1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -2030,7 +2140,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2076,6 +2186,11 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -2091,7 +2206,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2137,6 +2252,11 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
@@ -2152,6 +2272,57 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2163,295 +2334,259 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>sequences</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sources</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>primers</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>files</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sseqid</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>start_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>end_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>percent_identity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>full_length_of_feature_in_db</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>length_of_found_feature</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>percent_match_length</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fragment</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>database</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>annotation_tool</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>annotation_tool_version</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>annotation_report</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>input</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
         <is>
           <t>output_name</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequences</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sources</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>primers</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>files</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sseqid</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>start_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>end_location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>strand</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>percent_identity</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>full_length_of_feature_in_db</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>length_of_found_feature</t>
-        </is>
-      </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>percent_match_length</t>
+          <t>database_id</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>fragment</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>database</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Feature</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>annotation_tool</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>annotation_tool_version</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>annotation_report</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -2473,7 +2608,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2503,6 +2638,11 @@
         </is>
       </c>
       <c r="E1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -2683,7 +2823,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2738,6 +2878,11 @@
         </is>
       </c>
       <c r="J1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
         <is>
           <t>id</t>
         </is>

</xml_diff>

<commit_message>
remove camelcase from addgene
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -20,7 +20,7 @@
     <sheet name="ManuallyTypedSource" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="UploadedFileSource" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="RepositoryIdSource" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="AddGeneIdSource" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="AddgeneIdSource" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="WekWikGeneIdSource" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="SEVASource" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="BenchlingUrlSource" sheetId="17" state="visible" r:id="rId17"/>
@@ -520,7 +520,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"OligoPair,AddGenePlasmid"</formula1>
+      <formula1>"OligoPair,AddgenePlasmid"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
remove camelcase from addgene (#38)
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -20,7 +20,7 @@
     <sheet name="ManuallyTypedSource" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="UploadedFileSource" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="RepositoryIdSource" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="AddGeneIdSource" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="AddgeneIdSource" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="WekWikGeneIdSource" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="SEVASource" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="BenchlingUrlSource" sheetId="17" state="visible" r:id="rId17"/>
@@ -520,7 +520,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"OligoPair,AddGenePlasmid"</formula1>
+      <formula1>"OligoPair,AddgenePlasmid"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add classes for https://github.com/manulera/OpenCloning_backend/issues/296 and https://github.com/manulera/OpenCloning_backend/issues/295
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -39,18 +39,20 @@
     <sheet name="GibsonAssemblySource" sheetId="30" state="visible" r:id="rId30"/>
     <sheet name="InFusionSource" sheetId="31" state="visible" r:id="rId31"/>
     <sheet name="OverlapExtensionPCRLigationSource" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="GatewaySource" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="CRISPRSource" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="OligoHybridizationSource" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="CloningStrategy" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="AnnotationReport" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="PlannotateAnnotationReport" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="AnnotationSource" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="ReverseComplementSource" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="AssociatedFile" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="SequencingFile" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="InVivoAssemblySource" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="GatewaySource" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="CreLoxRecombinationSource" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="CRISPRSource" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="OligoHybridizationSource" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="CloningStrategy" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="AnnotationReport" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="PlannotateAnnotationReport" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="AnnotationSource" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="ReverseComplementSource" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="AssociatedFile" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="SequencingFile" sheetId="46" state="visible" r:id="rId46"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2050,6 +2052,67 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2110,7 +2173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2186,7 +2249,68 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2252,7 +2376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2318,7 +2442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2369,7 +2493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2386,6 +2510,52 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>sequences</t>
         </is>
       </c>
@@ -2415,7 +2585,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2441,137 +2611,91 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sseqid</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>start_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>end_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>percent_identity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>full_length_of_feature_in_db</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>length_of_found_feature</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>percent_match_length</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fragment</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>database</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
         <is>
           <t>sequence</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sseqid</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>start_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>end_location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>strand</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>percent_identity</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>full_length_of_feature_in_db</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>length_of_found_feature</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>percent_match_length</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>fragment</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>database</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Feature</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
       <c r="O1" t="inlineStr">
         <is>
           <t>type</t>
@@ -2583,7 +2707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2654,7 +2778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2705,7 +2829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2751,7 +2875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
add classes for https://github.com/manulera/OpenCloning_backend/issues/296 and https://github.com/manulera/OpenCloning_backend/issues/295 (#42)
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -39,18 +39,20 @@
     <sheet name="GibsonAssemblySource" sheetId="30" state="visible" r:id="rId30"/>
     <sheet name="InFusionSource" sheetId="31" state="visible" r:id="rId31"/>
     <sheet name="OverlapExtensionPCRLigationSource" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="GatewaySource" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="CRISPRSource" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="OligoHybridizationSource" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="CloningStrategy" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="AnnotationReport" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="PlannotateAnnotationReport" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="AnnotationSource" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="ReverseComplementSource" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="AssociatedFile" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="SequencingFile" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="InVivoAssemblySource" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="GatewaySource" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="CreLoxRecombinationSource" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="CRISPRSource" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="OligoHybridizationSource" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="CloningStrategy" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="AnnotationReport" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="PlannotateAnnotationReport" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="AnnotationSource" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="ReverseComplementSource" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="AssociatedFile" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="SequencingFile" sheetId="46" state="visible" r:id="rId46"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2050,6 +2052,67 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2110,7 +2173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2186,7 +2249,68 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2252,7 +2376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2318,7 +2442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2369,7 +2493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2386,6 +2510,52 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>sequences</t>
         </is>
       </c>
@@ -2415,7 +2585,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2441,137 +2611,91 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sseqid</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>start_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>end_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>percent_identity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>full_length_of_feature_in_db</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>length_of_found_feature</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>percent_match_length</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fragment</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>database</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
         <is>
           <t>sequence</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sseqid</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>start_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>end_location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>strand</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>percent_identity</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>full_length_of_feature_in_db</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>length_of_found_feature</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>percent_match_length</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>fragment</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>database</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Feature</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
       <c r="O1" t="inlineStr">
         <is>
           <t>type</t>
@@ -2583,7 +2707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2654,7 +2778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2705,7 +2829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2751,7 +2875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
coords within file (#43)
* coords within file https://github.com/manulera/OpenCloning_backend/issues/298

* run make

* correct 0-based
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -606,7 +606,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -637,30 +637,35 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>coordinates</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>input</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>output_name</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>database_id</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>id</t>
         </is>

</xml_diff>

<commit_message>
include versions in cloningstrategy
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -2550,7 +2550,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2582,6 +2582,21 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>files</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>schema_version</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>backend_version</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>frontend_version</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update linkml and add version to model (#46)
* update linkml

* include versions in cloningstrategy

* add versioning
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -2550,7 +2550,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2582,6 +2582,21 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>files</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>schema_version</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>backend_version</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>frontend_version</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Coordinates as text (#47)
* model changes

* remove unused files

* add migration + tests + better docs
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -30,29 +30,28 @@
     <sheet name="GenomeCoordinatesSource" sheetId="21" state="visible" r:id="rId21"/>
     <sheet name="SequenceCutSource" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="RestrictionEnzymeDigestionSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="SimpleSequenceLocation" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="AssemblyFragment" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="AssemblySource" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="PCRSource" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="LigationSource" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="HomologousRecombinationSource" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="GibsonAssemblySource" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="InFusionSource" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="OverlapExtensionPCRLigationSource" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="InVivoAssemblySource" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="GatewaySource" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="CreLoxRecombinationSource" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="CRISPRSource" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="OligoHybridizationSource" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="CloningStrategy" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="AnnotationReport" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="PlannotateAnnotationReport" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="AnnotationSource" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="ReverseComplementSource" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="AssociatedFile" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet name="SequencingFile" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="AssemblyFragment" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="AssemblySource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="PCRSource" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="LigationSource" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="HomologousRecombinationSource" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="GibsonAssemblySource" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="InFusionSource" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="OverlapExtensionPCRLigationSource" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="InVivoAssemblySource" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="GatewaySource" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="CreLoxRecombinationSource" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="CRISPRSource" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="OligoHybridizationSource" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="CloningStrategy" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="AnnotationReport" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="PlannotateAnnotationReport" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="AnnotationSource" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="ReverseComplementSource" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="AssociatedFile" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="SequencingFile" sheetId="45" state="visible" r:id="rId45"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1492,28 +1491,33 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>start</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>end</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>strand</t>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>left_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>right_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>reverse_complemented</t>
         </is>
       </c>
     </row>
@@ -1528,33 +1532,53 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>left_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>right_location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>reverse_complemented</t>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
         </is>
       </c>
     </row>
@@ -1569,6 +1593,72 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>add_primer_features</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1614,72 +1704,6 @@
         </is>
       </c>
       <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>add_primer_features</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -2057,51 +2081,56 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>restriction_enzymes</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>assembly</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>input</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>output</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
         <is>
           <t>output_name</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>database_id</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -2113,72 +2142,6 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>restriction_enzymes</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2254,12 +2217,256 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>guides</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>overhang_crick_3prime</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>forward_oligo</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>reverse_oligo</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2271,356 +2478,208 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
+          <t>sequences</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sources</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>primers</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>files</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>schema_version</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>backend_version</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>frontend_version</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>database_id</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sseqid</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>start_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>end_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>percent_identity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>full_length_of_feature_in_db</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>length_of_found_feature</t>
+        </is>
+      </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>guides</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>assembly</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>database_id</t>
+          <t>percent_match_length</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>overhang_crick_3prime</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>forward_oligo</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>reverse_oligo</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+          <t>fragment</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>database</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
         <is>
           <t>sequence</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequences</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sources</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>primers</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>files</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>schema_version</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>backend_version</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>frontend_version</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
@@ -2632,102 +2691,6 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sseqid</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>start_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>end_location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>strand</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>percent_identity</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>full_length_of_feature_in_db</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>length_of_found_feature</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>percent_match_length</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>fragment</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>database</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Feature</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2798,58 +2761,58 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2895,7 +2858,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
allow any type of SourceInput in AssemblySource
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -1520,27 +1520,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -1576,27 +1576,27 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>database_id</t>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>input</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -1627,27 +1627,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -1678,27 +1678,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -1785,27 +1785,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -1836,27 +1836,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -1887,27 +1887,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -1938,27 +1938,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -1994,27 +1994,27 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>database_id</t>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>input</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -2055,27 +2055,27 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>database_id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>database_id</t>
+          <t>input</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
@@ -2111,27 +2111,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -2162,27 +2162,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">

</xml_diff>

<commit_message>
include Open-DNA-Collections and switch to python
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -28,31 +28,32 @@
     <sheet name="SnapGenePlasmidSource" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="EuroscarfSource" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="IGEMSource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="SequenceCutSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="RestrictionEnzymeDigestionSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="AssemblyFragment" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="AssemblySource" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="PCRSource" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="LigationSource" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="HomologousRecombinationSource" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="GibsonAssemblySource" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="InFusionSource" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="OverlapExtensionPCRLigationSource" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="InVivoAssemblySource" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="GatewaySource" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="CreLoxRecombinationSource" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="CRISPRSource" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="OligoHybridizationSource" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="CloningStrategy" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="AnnotationReport" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="PlannotateAnnotationReport" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="AnnotationSource" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="ReverseComplementSource" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="AssociatedFile" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet name="SequencingFile" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="OpenDNACollectionsSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="SequenceCutSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="AssemblyFragment" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="AssemblySource" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="PCRSource" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="LigationSource" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="HomologousRecombinationSource" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="GibsonAssemblySource" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="InFusionSource" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="OverlapExtensionPCRLigationSource" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="InVivoAssemblySource" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="GatewaySource" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="CreLoxRecombinationSource" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="CRISPRSource" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="OligoHybridizationSource" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="CloningStrategy" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="AnnotationReport" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="PlannotateAnnotationReport" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="AnnotationSource" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="ReverseComplementSource" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="AssociatedFile" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="SequencingFile" sheetId="47" state="visible" r:id="rId47"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -761,7 +762,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -835,7 +836,7 @@
       <formula1>"depositor-full,addgene-full"</formula1>
     </dataValidation>
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -901,7 +902,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -967,7 +968,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1028,7 +1029,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1089,7 +1090,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1191,7 +1192,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1257,7 +1258,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1270,6 +1271,72 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequence_file_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>repository_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1345,7 +1412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1401,7 +1468,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1457,7 +1524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1503,7 +1570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1554,7 +1621,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1600,57 +1667,6 @@
         </is>
       </c>
       <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1978,6 +1994,57 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2028,7 +2095,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2094,7 +2161,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2145,7 +2212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2196,7 +2263,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2247,7 +2314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2264,36 +2331,36 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2310,207 +2377,207 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequences</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sources</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>primers</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>files</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>schema_version</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>backend_version</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>frontend_version</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sseqid</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>start_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>end_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>percent_identity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>full_length_of_feature_in_db</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>length_of_found_feature</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>percent_match_length</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fragment</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>database</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
         <is>
           <t>sequence</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequences</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sources</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>primers</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>files</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>schema_version</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>backend_version</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>frontend_version</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sseqid</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>start_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>end_location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>strand</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>percent_identity</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>full_length_of_feature_in_db</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>length_of_found_feature</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>percent_match_length</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>fragment</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>database</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Feature</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
       <c r="O1" t="inlineStr">
         <is>
           <t>type</t>
@@ -2522,7 +2589,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2588,7 +2655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2634,7 +2701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2680,7 +2747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
include Open-DNA-Collections and switch to python (#61)
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -28,31 +28,32 @@
     <sheet name="SnapGenePlasmidSource" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="EuroscarfSource" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="IGEMSource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="SequenceCutSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="RestrictionEnzymeDigestionSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="AssemblyFragment" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="AssemblySource" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="PCRSource" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="LigationSource" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="HomologousRecombinationSource" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="GibsonAssemblySource" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="InFusionSource" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="OverlapExtensionPCRLigationSource" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="InVivoAssemblySource" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="GatewaySource" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="CreLoxRecombinationSource" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="CRISPRSource" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="OligoHybridizationSource" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="CloningStrategy" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="AnnotationReport" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="PlannotateAnnotationReport" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="AnnotationSource" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="ReverseComplementSource" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="AssociatedFile" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet name="SequencingFile" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="OpenDNACollectionsSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="SequenceCutSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="AssemblyFragment" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="AssemblySource" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="PCRSource" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="LigationSource" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="HomologousRecombinationSource" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="GibsonAssemblySource" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="InFusionSource" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="OverlapExtensionPCRLigationSource" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="InVivoAssemblySource" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="GatewaySource" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="CreLoxRecombinationSource" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="CRISPRSource" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="OligoHybridizationSource" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="CloningStrategy" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="AnnotationReport" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="PlannotateAnnotationReport" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="AnnotationSource" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="ReverseComplementSource" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="AssociatedFile" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="SequencingFile" sheetId="47" state="visible" r:id="rId47"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -761,7 +762,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -835,7 +836,7 @@
       <formula1>"depositor-full,addgene-full"</formula1>
     </dataValidation>
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -901,7 +902,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -967,7 +968,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1028,7 +1029,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1089,7 +1090,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1191,7 +1192,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1257,7 +1258,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva"</formula1>
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1270,6 +1271,72 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequence_file_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>repository_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1345,7 +1412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1401,7 +1468,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1457,7 +1524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1503,7 +1570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1554,7 +1621,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1600,57 +1667,6 @@
         </is>
       </c>
       <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1978,6 +1994,57 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2028,7 +2095,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2094,7 +2161,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2145,7 +2212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2196,7 +2263,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2247,7 +2314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2264,36 +2331,36 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2310,207 +2377,207 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequences</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sources</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>primers</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>files</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>schema_version</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>backend_version</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>frontend_version</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sseqid</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>start_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>end_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>percent_identity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>full_length_of_feature_in_db</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>length_of_found_feature</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>percent_match_length</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fragment</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>database</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
         <is>
           <t>sequence</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequences</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sources</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>primers</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>files</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>schema_version</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>backend_version</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>frontend_version</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sseqid</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>start_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>end_location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>strand</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>percent_identity</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>full_length_of_feature_in_db</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>length_of_found_feature</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>percent_match_length</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>fragment</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>database</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Feature</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
       <c r="O1" t="inlineStr">
         <is>
           <t>type</t>
@@ -2522,7 +2589,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2588,7 +2655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2634,7 +2701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2680,7 +2747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
model changed for #70
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -29,31 +29,32 @@
     <sheet name="EuroscarfSource" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="IGEMSource" sheetId="21" state="visible" r:id="rId21"/>
     <sheet name="OpenDNACollectionsSource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="SequenceCutSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="RestrictionEnzymeDigestionSource" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="AssemblyFragment" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="AssemblySource" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="PCRSource" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="LigationSource" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="HomologousRecombinationSource" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="GibsonAssemblySource" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="InFusionSource" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="OverlapExtensionPCRLigationSource" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="InVivoAssemblySource" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="GatewaySource" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="CreLoxRecombinationSource" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="CRISPRSource" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="OligoHybridizationSource" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="CloningStrategy" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="AnnotationReport" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="PlannotateAnnotationReport" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="AnnotationSource" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="ReverseComplementSource" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet name="AssociatedFile" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet name="SequencingFile" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="NCBISequenceSource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="SequenceCutSource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="AssemblyFragment" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="AssemblySource" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="PCRSource" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="LigationSource" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="HomologousRecombinationSource" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="GibsonAssemblySource" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="InFusionSource" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="OverlapExtensionPCRLigationSource" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="InVivoAssemblySource" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="GatewaySource" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="CreLoxRecombinationSource" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="CRISPRSource" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="OligoHybridizationSource" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="CloningStrategy" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="AnnotationReport" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="PlannotateAnnotationReport" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="AnnotationSource" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="ReverseComplementSource" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="AssociatedFile" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="SequencingFile" sheetId="48" state="visible" r:id="rId48"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -572,56 +573,36 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>overhang_crick_3prime</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>overhang_watson_3prime</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>user_input</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1337,7 +1318,73 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>repository_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1353,66 +1400,66 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>sequence_accession</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
           <t>locus_tag</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>gene_id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>start</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>end</t>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>repository_name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>strand</t>
+          <t>type</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>type</t>
+          <t>output_name</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>output_name</t>
+          <t>database_id</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>database_id</t>
+          <t>input</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1468,7 +1515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1524,7 +1571,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1570,7 +1617,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1621,7 +1668,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1667,57 +1714,6 @@
         </is>
       </c>
       <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -2045,6 +2041,57 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2095,7 +2142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2161,7 +2208,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2212,7 +2259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2263,7 +2310,53 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2314,7 +2407,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2331,253 +2424,207 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequences</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sources</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>primers</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>files</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>schema_version</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>backend_version</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>frontend_version</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sseqid</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>start_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>end_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>percent_identity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>full_length_of_feature_in_db</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>length_of_found_feature</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>percent_match_length</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fragment</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>database</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
         <is>
           <t>sequence</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequences</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sources</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>primers</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>files</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>schema_version</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>backend_version</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>frontend_version</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sseqid</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>start_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>end_location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>strand</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>percent_identity</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>full_length_of_feature_in_db</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>length_of_found_feature</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>percent_match_length</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>fragment</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>database</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Feature</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
       <c r="O1" t="inlineStr">
         <is>
           <t>type</t>
@@ -2589,7 +2636,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2655,7 +2702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2701,7 +2748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2747,7 +2794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
rename location to coordinates
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -1329,7 +1329,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>location</t>
+          <t>coordinates</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1410,7 +1410,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>location</t>
+          <t>coordinates</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">

</xml_diff>

<commit_message>
add manually typed sequence as class
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -10,51 +10,52 @@
     <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="TemplateSequence" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="TextFileSequence" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Primer" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="SourceInput" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="SequenceCut" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="RestrictionSequenceCut" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="DatabaseSource" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="CollectionSource" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="CollectionOption" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="CollectionOptionInfo" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="ManuallyTypedSource" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="UploadedFileSource" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="RepositoryIdSource" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="AddgeneIdSource" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="WekWikGeneIdSource" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="SEVASource" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="BenchlingUrlSource" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="SnapGenePlasmidSource" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="EuroscarfSource" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="IGEMSource" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="OpenDNACollectionsSource" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="NCBISequenceSource" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="GenomeCoordinatesSource" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="SequenceCutSource" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="RestrictionEnzymeDigestionSource" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="AssemblyFragment" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="AssemblySource" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="PCRSource" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="LigationSource" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="HomologousRecombinationSource" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="GibsonAssemblySource" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="InFusionSource" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="OverlapExtensionPCRLigationSource" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="InVivoAssemblySource" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="RestrictionAndLigationSource" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="GatewaySource" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="CreLoxRecombinationSource" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="CRISPRSource" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="OligoHybridizationSource" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="PolymeraseExtensionSource" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="CloningStrategy" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="AnnotationReport" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="PlannotateAnnotationReport" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="AnnotationSource" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet name="ReverseComplementSource" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet name="AssociatedFile" sheetId="47" state="visible" r:id="rId47"/>
-    <sheet name="SequencingFile" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="ManuallyTypedSequence" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Primer" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="SourceInput" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="SequenceCut" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="RestrictionSequenceCut" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="DatabaseSource" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="CollectionSource" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="CollectionOption" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="CollectionOptionInfo" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="ManuallyTypedSource" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="UploadedFileSource" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="RepositoryIdSource" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="AddgeneIdSource" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="WekWikGeneIdSource" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="SEVASource" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="BenchlingUrlSource" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="SnapGenePlasmidSource" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="EuroscarfSource" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="IGEMSource" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="OpenDNACollectionsSource" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="NCBISequenceSource" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="GenomeCoordinatesSource" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="SequenceCutSource" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="RestrictionEnzymeDigestionSource" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="AssemblyFragment" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="AssemblySource" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="PCRSource" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="LigationSource" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="HomologousRecombinationSource" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="GibsonAssemblySource" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="InFusionSource" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="OverlapExtensionPCRLigationSource" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="InVivoAssemblySource" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="RestrictionAndLigationSource" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="GatewaySource" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="CreLoxRecombinationSource" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="CRISPRSource" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="OligoHybridizationSource" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="PolymeraseExtensionSource" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="CloningStrategy" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="AnnotationReport" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="PlannotateAnnotationReport" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="AnnotationSource" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="ReverseComplementSource" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="AssociatedFile" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="SequencingFile" sheetId="49" state="visible" r:id="rId49"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -486,6 +487,77 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>category_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>options</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -516,7 +588,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -567,7 +639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -613,7 +685,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -689,7 +761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -750,7 +822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -824,7 +896,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -890,7 +962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -956,7 +1028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1017,7 +1089,48 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>primer_design</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1078,48 +1191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>primer_design</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1180,7 +1252,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1246,7 +1318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1312,7 +1384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1378,7 +1450,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1459,7 +1531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1515,7 +1587,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1571,7 +1643,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1617,7 +1689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1658,62 +1730,6 @@
         </is>
       </c>
       <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>add_primer_features</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -1786,6 +1802,62 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>add_primer_features</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1831,7 +1903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1882,7 +1954,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1933,7 +2005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1984,7 +2056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2035,7 +2107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2086,7 +2158,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2142,7 +2214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2208,7 +2280,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2259,7 +2331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2276,41 +2348,143 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>overhang_crick_3prime</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>overhang_watson_3prime</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>circular</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>overhang_crick_3prime</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2327,304 +2501,207 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+          <t>type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequences</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sources</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>primers</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>files</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>schema_version</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>backend_version</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>frontend_version</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sseqid</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>start_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>end_location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>strand</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>percent_identity</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>full_length_of_feature_in_db</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>length_of_found_feature</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>percent_match_length</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>fragment</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>database</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Feature</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
         <is>
           <t>sequence</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>overhang_crick_3prime</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequences</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sources</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>primers</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>files</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>schema_version</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>backend_version</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>frontend_version</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sseqid</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>start_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>end_location</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>strand</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>percent_identity</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>full_length_of_feature_in_db</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>length_of_found_feature</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>percent_match_length</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>fragment</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>database</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Feature</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>sequence</t>
-        </is>
-      </c>
       <c r="O1" t="inlineStr">
         <is>
           <t>type</t>
@@ -2636,7 +2713,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2702,7 +2779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2748,7 +2825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2794,7 +2871,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2851,6 +2928,52 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sequence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2876,7 +2999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2907,7 +3030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2943,7 +3066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2987,75 +3110,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>category_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>image</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>options</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
remove field repository_name and revert examples
</commit_message>
<xml_diff>
--- a/project/excel/opencloning_linkml.xlsx
+++ b/project/excel/opencloning_linkml.xlsx
@@ -767,7 +767,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -783,114 +783,96 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>repository_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>input</t>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequence_file_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>addgene_sequence_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>database_id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequence_file_url</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>addgene_sequence_type</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>repository_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"depositor-full,addgene-full"</formula1>
     </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -902,7 +884,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -923,610 +905,520 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>repository_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>database_id</t>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>input</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>input</t>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequence_file_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>circular</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>primer_design</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequence_file_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sequence_file_url</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>coordinates</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>output_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>database_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>assembly_accession</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>locus_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>gene_id</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>coordinates</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>repository_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>output_name</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequence_file_url</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>repository_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>repository_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>circular</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>primer_design</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>repository_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>repository_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequence_file_url</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>repository_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>sequence_file_url</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>repository_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>coordinates</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>repository_name</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>output_name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>database_id</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>assembly_accession</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>locus_tag</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>gene_id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>coordinates</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>repository_id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>repository_name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>output_name</t>
+          <t>database_id</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>database_id</t>
+          <t>input</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>input</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"addgene,genbank,benchling,snapgene,euroscarf,igem,wekwikgene,seva,open_dna_collections"</formula1>
-    </dataValidation>
-  </dataValidations>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>